<commit_message>
Soft switching conditions are defined. Test procedure is developed.
</commit_message>
<xml_diff>
--- a/Buck Converter/Soldering & Test Procedure.xlsx
+++ b/Buck Converter/Soldering & Test Procedure.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="421">
   <si>
     <t>SOLDER</t>
   </si>
@@ -1228,6 +1228,66 @@
   </si>
   <si>
     <t>5V / 3V3</t>
+  </si>
+  <si>
+    <t>HALF BRIDGE TESTS</t>
+  </si>
+  <si>
+    <t>Verification of Soft Turn-off</t>
+  </si>
+  <si>
+    <t>Soft Turn-off</t>
+  </si>
+  <si>
+    <t>Low DCV, Single Brg., DPT</t>
+  </si>
+  <si>
+    <t>Vgs Waveform</t>
+  </si>
+  <si>
+    <t>Verification of SCP Signal Generation</t>
+  </si>
+  <si>
+    <t>dI/dt creation</t>
+  </si>
+  <si>
+    <t>Verification of SC Protection Mechanism</t>
+  </si>
+  <si>
+    <t>Safe Turn-off</t>
+  </si>
+  <si>
+    <t>Low DCV, Double Brg., DPT</t>
+  </si>
+  <si>
+    <t>Vgs Waveforms</t>
+  </si>
+  <si>
+    <t>Vgs Waveform Obs.</t>
+  </si>
+  <si>
+    <t>9V, 5V Waveform Obs</t>
+  </si>
+  <si>
+    <t>DC Voltages</t>
+  </si>
+  <si>
+    <t>Mid DCV, Double Brg., DPT</t>
+  </si>
+  <si>
+    <t>Mid DCV, Single Brg., DPT</t>
+  </si>
+  <si>
+    <t>Half Bridge -1</t>
+  </si>
+  <si>
+    <t>Half Bridge -2</t>
+  </si>
+  <si>
+    <t>Vds Waveform</t>
+  </si>
+  <si>
+    <t>BUCK CONVERTER TESTS</t>
   </si>
 </sst>
 </file>
@@ -1935,8 +1995,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B22:F227" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B22:F227"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="B22:F230" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B22:F230"/>
   <tableColumns count="5">
     <tableColumn id="1" name="BUT"/>
     <tableColumn id="2" name="Test"/>
@@ -6418,10 +6478,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="N61" sqref="N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6429,7 +6489,7 @@
     <col min="1" max="1" width="3" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" customWidth="1"/>
   </cols>
@@ -6641,9 +6701,6 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>1</v>
-      </c>
       <c r="B21" s="45"/>
       <c r="C21" s="45" t="s">
         <v>368</v>
@@ -6814,7 +6871,7 @@
       <c r="E32" s="44"/>
       <c r="F32" s="44"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="46"/>
       <c r="B33" t="s">
         <v>350</v>
@@ -6829,7 +6886,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="46"/>
       <c r="B34" t="s">
         <v>350</v>
@@ -6844,7 +6901,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="46"/>
       <c r="B35" t="s">
         <v>350</v>
@@ -6859,7 +6916,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="46"/>
       <c r="B36" t="s">
         <v>350</v>
@@ -6874,7 +6931,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="46"/>
       <c r="B37" t="s">
         <v>350</v>
@@ -6889,7 +6946,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="46"/>
       <c r="B38" t="s">
         <v>350</v>
@@ -6904,7 +6961,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="46"/>
       <c r="B39" t="s">
         <v>350</v>
@@ -6919,7 +6976,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="46"/>
       <c r="B40" t="s">
         <v>350</v>
@@ -6934,7 +6991,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="46"/>
       <c r="B41" t="s">
         <v>350</v>
@@ -6949,7 +7006,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="46"/>
       <c r="B42" t="s">
         <v>350</v>
@@ -6964,7 +7021,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="46"/>
       <c r="B43" t="s">
         <v>350</v>
@@ -6979,7 +7036,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="46"/>
       <c r="B44" t="s">
         <v>350</v>
@@ -6994,7 +7051,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="46"/>
       <c r="B45" t="s">
         <v>350</v>
@@ -7008,6 +7065,357 @@
       <c r="E45" t="s">
         <v>397</v>
       </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="44"/>
+      <c r="C46" s="44" t="s">
+        <v>401</v>
+      </c>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="42"/>
+      <c r="B47" t="s">
+        <v>417</v>
+      </c>
+      <c r="C47" t="s">
+        <v>404</v>
+      </c>
+      <c r="D47" t="s">
+        <v>378</v>
+      </c>
+      <c r="E47" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="42"/>
+      <c r="B48" t="s">
+        <v>417</v>
+      </c>
+      <c r="C48" t="s">
+        <v>402</v>
+      </c>
+      <c r="D48" t="s">
+        <v>378</v>
+      </c>
+      <c r="E48" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="42"/>
+      <c r="B49" t="s">
+        <v>417</v>
+      </c>
+      <c r="C49" t="s">
+        <v>406</v>
+      </c>
+      <c r="D49" t="s">
+        <v>378</v>
+      </c>
+      <c r="E49" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="42"/>
+      <c r="B50" t="s">
+        <v>417</v>
+      </c>
+      <c r="C50" t="s">
+        <v>408</v>
+      </c>
+      <c r="D50" t="s">
+        <v>378</v>
+      </c>
+      <c r="E50" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="42"/>
+      <c r="B51" t="s">
+        <v>417</v>
+      </c>
+      <c r="C51" t="s">
+        <v>416</v>
+      </c>
+      <c r="D51" t="s">
+        <v>378</v>
+      </c>
+      <c r="E51" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="42"/>
+      <c r="B52" t="s">
+        <v>417</v>
+      </c>
+      <c r="C52" t="s">
+        <v>416</v>
+      </c>
+      <c r="D52" t="s">
+        <v>378</v>
+      </c>
+      <c r="E52" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="42"/>
+      <c r="B53" t="s">
+        <v>417</v>
+      </c>
+      <c r="C53" t="s">
+        <v>410</v>
+      </c>
+      <c r="D53" t="s">
+        <v>412</v>
+      </c>
+      <c r="E53" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="42"/>
+      <c r="B54" t="s">
+        <v>417</v>
+      </c>
+      <c r="C54" t="s">
+        <v>410</v>
+      </c>
+      <c r="D54" t="s">
+        <v>413</v>
+      </c>
+      <c r="E54" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="42"/>
+      <c r="B55" t="s">
+        <v>417</v>
+      </c>
+      <c r="C55" t="s">
+        <v>415</v>
+      </c>
+      <c r="D55" t="s">
+        <v>412</v>
+      </c>
+      <c r="E55" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="42"/>
+      <c r="B56" t="s">
+        <v>417</v>
+      </c>
+      <c r="C56" t="s">
+        <v>415</v>
+      </c>
+      <c r="D56" t="s">
+        <v>378</v>
+      </c>
+      <c r="E56" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="42"/>
+      <c r="B57" t="s">
+        <v>417</v>
+      </c>
+      <c r="C57" t="s">
+        <v>415</v>
+      </c>
+      <c r="D57" t="s">
+        <v>413</v>
+      </c>
+      <c r="E57" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="42"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="42"/>
+      <c r="B59" t="s">
+        <v>418</v>
+      </c>
+      <c r="C59" t="s">
+        <v>404</v>
+      </c>
+      <c r="D59" t="s">
+        <v>378</v>
+      </c>
+      <c r="E59" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="42"/>
+      <c r="B60" t="s">
+        <v>418</v>
+      </c>
+      <c r="C60" t="s">
+        <v>402</v>
+      </c>
+      <c r="D60" t="s">
+        <v>378</v>
+      </c>
+      <c r="E60" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="42"/>
+      <c r="B61" t="s">
+        <v>418</v>
+      </c>
+      <c r="C61" t="s">
+        <v>406</v>
+      </c>
+      <c r="D61" t="s">
+        <v>378</v>
+      </c>
+      <c r="E61" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="42"/>
+      <c r="B62" t="s">
+        <v>418</v>
+      </c>
+      <c r="C62" t="s">
+        <v>408</v>
+      </c>
+      <c r="D62" t="s">
+        <v>378</v>
+      </c>
+      <c r="E62" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="42"/>
+      <c r="B63" t="s">
+        <v>418</v>
+      </c>
+      <c r="C63" t="s">
+        <v>416</v>
+      </c>
+      <c r="D63" t="s">
+        <v>378</v>
+      </c>
+      <c r="E63" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="42"/>
+      <c r="B64" t="s">
+        <v>418</v>
+      </c>
+      <c r="C64" t="s">
+        <v>416</v>
+      </c>
+      <c r="D64" t="s">
+        <v>378</v>
+      </c>
+      <c r="E64" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="42"/>
+      <c r="B65" t="s">
+        <v>418</v>
+      </c>
+      <c r="C65" t="s">
+        <v>410</v>
+      </c>
+      <c r="D65" t="s">
+        <v>412</v>
+      </c>
+      <c r="E65" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="42"/>
+      <c r="B66" t="s">
+        <v>418</v>
+      </c>
+      <c r="C66" t="s">
+        <v>410</v>
+      </c>
+      <c r="D66" t="s">
+        <v>413</v>
+      </c>
+      <c r="E66" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="42"/>
+      <c r="B67" t="s">
+        <v>418</v>
+      </c>
+      <c r="C67" t="s">
+        <v>415</v>
+      </c>
+      <c r="D67" t="s">
+        <v>412</v>
+      </c>
+      <c r="E67" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="42"/>
+      <c r="B68" t="s">
+        <v>418</v>
+      </c>
+      <c r="C68" t="s">
+        <v>415</v>
+      </c>
+      <c r="D68" t="s">
+        <v>378</v>
+      </c>
+      <c r="E68" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="42"/>
+      <c r="B69" t="s">
+        <v>418</v>
+      </c>
+      <c r="C69" t="s">
+        <v>415</v>
+      </c>
+      <c r="D69" t="s">
+        <v>413</v>
+      </c>
+      <c r="E69" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="44"/>
+      <c r="C70" s="44" t="s">
+        <v>420</v>
+      </c>
+      <c r="D70" s="44"/>
+      <c r="E70" s="44"/>
+      <c r="F70" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
@hakansrc ile DSP'ye giriş yapıldı.
</commit_message>
<xml_diff>
--- a/Buck Converter/Soldering & Test Procedure.xlsx
+++ b/Buck Converter/Soldering & Test Procedure.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="SOLDER" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="422">
   <si>
     <t>SOLDER</t>
   </si>
@@ -1288,6 +1288,9 @@
   </si>
   <si>
     <t>BUCK CONVERTER TESTS</t>
+  </si>
+  <si>
+    <t>Safe State (850V)</t>
   </si>
 </sst>
 </file>
@@ -2271,10 +2274,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:V151"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N88" sqref="N88"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6468,7 +6474,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -6480,8 +6486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="N61" sqref="N61"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6741,6 +6747,9 @@
       <c r="E23" t="s">
         <v>373</v>
       </c>
+      <c r="F23" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="42"/>
@@ -6756,6 +6765,9 @@
       <c r="E24" t="s">
         <v>373</v>
       </c>
+      <c r="F24" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="42"/>
@@ -6771,6 +6783,9 @@
       <c r="E25" t="s">
         <v>373</v>
       </c>
+      <c r="F25" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="43"/>
@@ -6786,6 +6801,9 @@
       <c r="E26" t="s">
         <v>373</v>
       </c>
+      <c r="F26" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="43"/>
@@ -6801,6 +6819,9 @@
       <c r="E27" t="s">
         <v>373</v>
       </c>
+      <c r="F27" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="43"/>
@@ -6816,6 +6837,9 @@
       <c r="E28" t="s">
         <v>373</v>
       </c>
+      <c r="F28" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="43"/>
@@ -6831,6 +6855,9 @@
       <c r="E29" t="s">
         <v>373</v>
       </c>
+      <c r="F29" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="43"/>
@@ -6846,6 +6873,9 @@
       <c r="E30" t="s">
         <v>373</v>
       </c>
+      <c r="F30" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="43"/>
@@ -6860,6 +6890,9 @@
       </c>
       <c r="E31" t="s">
         <v>373</v>
+      </c>
+      <c r="F31" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Important progress has been achieved on software: - PWM signals for Interleaved Buck Converter are generated successfully. - LED / Push Button / Enable Signal codes are completed. - DSP is able to understand and react to an overcurrent signal in just ~10 nsec. - Soft-turn-off and hard-turn-off mechanisms are fully integrated into code. - DPT pulses are generated. Instead of using microsecond delay function an assembly code is used and it does the job quite well.
The next step is reading analog signals as single channel or differential. @ozank
</commit_message>
<xml_diff>
--- a/Buck Converter/Soldering & Test Procedure.xlsx
+++ b/Buck Converter/Soldering & Test Procedure.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SOLDER" sheetId="1" r:id="rId1"/>
     <sheet name="TEST" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="430">
   <si>
     <t>SOLDER</t>
   </si>
@@ -1291,6 +1292,30 @@
   </si>
   <si>
     <t>Safe State (850V)</t>
+  </si>
+  <si>
+    <t>LED Driver is changed</t>
+  </si>
+  <si>
+    <t>DIN1 pin is changed</t>
+  </si>
+  <si>
+    <t>EN signalleri üretildi</t>
+  </si>
+  <si>
+    <t>Faz açısı ayarlanamadı, SW2'ye basınca fazda kayma oluyor</t>
+  </si>
+  <si>
+    <t>GPIO interrupt is which trigs STO with 10nsec delay</t>
+  </si>
+  <si>
+    <t>HTO is activated 250nsec after STO</t>
+  </si>
+  <si>
+    <t>No problem</t>
+  </si>
+  <si>
+    <t>The pulses are generated without any problem</t>
   </si>
 </sst>
 </file>
@@ -2279,7 +2304,7 @@
   </sheetPr>
   <dimension ref="A1:V151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -6486,8 +6511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6497,7 +6522,7 @@
     <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="53.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -6918,6 +6943,9 @@
       <c r="E33" t="s">
         <v>400</v>
       </c>
+      <c r="F33" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="46"/>
@@ -6948,6 +6976,9 @@
       <c r="E35" t="s">
         <v>379</v>
       </c>
+      <c r="F35" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="46"/>
@@ -6963,6 +6994,9 @@
       <c r="E36" t="s">
         <v>380</v>
       </c>
+      <c r="F36" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="46"/>
@@ -6978,6 +7012,9 @@
       <c r="E37" t="s">
         <v>382</v>
       </c>
+      <c r="F37" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="46"/>
@@ -6993,6 +7030,9 @@
       <c r="E38" t="s">
         <v>395</v>
       </c>
+      <c r="F38" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="46"/>
@@ -7008,6 +7048,9 @@
       <c r="E39" t="s">
         <v>387</v>
       </c>
+      <c r="F39" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="46"/>
@@ -7023,6 +7066,9 @@
       <c r="E40" t="s">
         <v>384</v>
       </c>
+      <c r="F40" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="46"/>
@@ -7097,6 +7143,9 @@
       </c>
       <c r="E45" t="s">
         <v>397</v>
+      </c>
+      <c r="F45" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
The software for OL control is fully completed with all phases.
</commit_message>
<xml_diff>
--- a/Buck Converter/Soldering & Test Procedure.xlsx
+++ b/Buck Converter/Soldering & Test Procedure.xlsx
@@ -16,7 +16,6 @@
     <sheet name="TEST" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="431">
   <si>
     <t>SOLDER</t>
   </si>
@@ -1316,6 +1315,9 @@
   </si>
   <si>
     <t>The pulses are generated without any problem</t>
+  </si>
+  <si>
+    <t>It is being measured without any problem</t>
   </si>
 </sst>
 </file>
@@ -6512,7 +6514,7 @@
   <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7084,6 +7086,9 @@
       <c r="E41" t="s">
         <v>390</v>
       </c>
+      <c r="F41" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="46"/>
@@ -7099,6 +7104,9 @@
       <c r="E42" t="s">
         <v>390</v>
       </c>
+      <c r="F42" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="46"/>
@@ -7114,6 +7122,9 @@
       <c r="E43" t="s">
         <v>390</v>
       </c>
+      <c r="F43" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="46"/>
@@ -7128,6 +7139,9 @@
       </c>
       <c r="E44" t="s">
         <v>390</v>
+      </c>
+      <c r="F44" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>